<commit_message>
Change the test question
</commit_message>
<xml_diff>
--- a/percentage_result.xlsx
+++ b/percentage_result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,10 +424,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>25% of 2000</t>
         </is>
       </c>
-      <c r="B1" t="n">
+      <c r="B2" t="n">
         <v>500</v>
       </c>
     </row>

</xml_diff>